<commit_message>
se comentaron todos los datos y se añadio readme y requirements
</commit_message>
<xml_diff>
--- a/Desafio/data/covid_colombia_100.xlsx
+++ b/Desafio/data/covid_colombia_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\equipo\code\universidad\tecnicas de programacion\Desafio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094F1539-57AD-4364-A5F9-E002B0D4458D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71ABE74-4035-4F05-98E0-FAA350E7E10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,7 +677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>